<commit_message>
Add registerTMALL and update write_xlsx
</commit_message>
<xml_diff>
--- a/files/member_SR_TNF_1.xlsx
+++ b/files/member_SR_TNF_1.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">sheet1!$A$1:$I$1332</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6665" uniqueCount="3544">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6700" uniqueCount="3552">
   <si>
     <t>S21013880</t>
   </si>
@@ -10663,6 +10664,38 @@
   </si>
   <si>
     <t>mobile</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>S21000847</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>S21000847</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>tnf.demo.7709</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NF0A2VEONYB100S</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NF00A7LNJK3100M</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NF0A2XY8DGP100M</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NF0A32YNTES1060</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NF0A2UCLJK31XXLREG</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -11637,8 +11670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1321" workbookViewId="0">
-      <selection activeCell="E1339" sqref="E1339"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="A1:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -11694,7 +11727,7 @@
         <v>1844</v>
       </c>
       <c r="C2" t="s">
-        <v>75</v>
+        <v>3544</v>
       </c>
       <c r="D2" t="s">
         <v>77</v>
@@ -54276,6 +54309,220 @@
       </c>
       <c r="J1332" t="s">
         <v>2898</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="19.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>3534</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3535</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>3536</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3537</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3538</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>3539</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3540</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3541</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>3542</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3543</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3546</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3545</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3547</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>698</v>
+      </c>
+      <c r="G2">
+        <v>698</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>698</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2762</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3548</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>298</v>
+      </c>
+      <c r="G3">
+        <v>298</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>298</v>
+      </c>
+      <c r="J3" t="s">
+        <v>2762</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3549</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>88</v>
+      </c>
+      <c r="G4">
+        <v>62</v>
+      </c>
+      <c r="H4">
+        <v>26</v>
+      </c>
+      <c r="I4">
+        <v>88</v>
+      </c>
+      <c r="J4" t="s">
+        <v>2762</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3550</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1098</v>
+      </c>
+      <c r="G5">
+        <v>549</v>
+      </c>
+      <c r="H5">
+        <v>549</v>
+      </c>
+      <c r="I5">
+        <v>1098</v>
+      </c>
+      <c r="J5" t="s">
+        <v>2762</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>1825</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1844</v>
+      </c>
+      <c r="C6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3551</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>498</v>
+      </c>
+      <c r="G6">
+        <v>498</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>498</v>
+      </c>
+      <c r="J6" t="s">
+        <v>2762</v>
       </c>
     </row>
   </sheetData>

</xml_diff>